<commit_message>
Testing - changes made
</commit_message>
<xml_diff>
--- a/src/php/dbscript/dbdataexcel.xlsx
+++ b/src/php/dbscript/dbdataexcel.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Apache24\htdocs\notflix\src\php\dbscript\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Apache24\htdocs\src\php\dbscript\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="UserAcct" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="37">
   <si>
     <t>UserID</t>
   </si>
@@ -115,66 +115,6 @@
   </si>
   <si>
     <t>src/php/videosrc/SRC-004.mp4</t>
-  </si>
-  <si>
-    <t>TRCK00002</t>
-  </si>
-  <si>
-    <t>TrackTwoTitle</t>
-  </si>
-  <si>
-    <t>Track 2 - Title - Description - testing</t>
-  </si>
-  <si>
-    <t>src/php/videosrc/SRC-002.mp4</t>
-  </si>
-  <si>
-    <t>TRCK00003</t>
-  </si>
-  <si>
-    <t>Track 3 Title</t>
-  </si>
-  <si>
-    <t>Track 3 - Title - Description</t>
-  </si>
-  <si>
-    <t>src/php/videosrc/SRC-003.mp4</t>
-  </si>
-  <si>
-    <t>TRCK00004</t>
-  </si>
-  <si>
-    <t>Track 4 Title</t>
-  </si>
-  <si>
-    <t>Track 4 - Title - Description</t>
-  </si>
-  <si>
-    <t>src/php/videosrc/SRC-00004.mp4</t>
-  </si>
-  <si>
-    <t>TRCK00005</t>
-  </si>
-  <si>
-    <t>testingvideo</t>
-  </si>
-  <si>
-    <t>testing video - video upload</t>
-  </si>
-  <si>
-    <t>src/php/videosrc/SRC-00006.mp4</t>
-  </si>
-  <si>
-    <t>TRCK00006</t>
-  </si>
-  <si>
-    <t>testingTrackVideo</t>
-  </si>
-  <si>
-    <t>Testing track video upload</t>
-  </si>
-  <si>
-    <t>src/php/videosrc/SRC-00007.mov</t>
   </si>
   <si>
     <t>QWRtaW4x</t>
@@ -202,6 +142,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -237,10 +180,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -523,8 +467,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -533,6 +477,8 @@
     <col min="4" max="4" width="11.85546875" customWidth="1"/>
     <col min="5" max="5" width="19.85546875" customWidth="1"/>
     <col min="6" max="6" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="14.28515625" customWidth="1"/>
     <col min="12" max="12" width="21" customWidth="1"/>
   </cols>
@@ -559,17 +505,17 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
       <c r="J1" t="s">
         <v>9</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>56</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -583,7 +529,7 @@
         <v>11</v>
       </c>
       <c r="E2" t="s">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="F2" t="s">
         <v>12</v>
@@ -591,17 +537,17 @@
       <c r="G2">
         <v>22221111</v>
       </c>
-      <c r="H2" s="1">
+      <c r="H2" s="3">
         <v>44276</v>
       </c>
-      <c r="I2" s="1">
+      <c r="I2" s="3">
         <v>44275</v>
       </c>
       <c r="J2" t="s">
         <v>11</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>53</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -615,22 +561,22 @@
         <v>14</v>
       </c>
       <c r="E3" t="s">
-        <v>51</v>
+        <v>31</v>
       </c>
       <c r="F3" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="1">
+      <c r="H3" s="3">
         <v>44279</v>
       </c>
-      <c r="I3" s="1">
+      <c r="I3" s="3">
         <v>44278</v>
       </c>
       <c r="J3" t="s">
         <v>16</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>54</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -644,7 +590,7 @@
         <v>18</v>
       </c>
       <c r="E4" t="s">
-        <v>52</v>
+        <v>32</v>
       </c>
       <c r="F4" t="s">
         <v>19</v>
@@ -652,17 +598,17 @@
       <c r="G4">
         <v>11112222</v>
       </c>
-      <c r="H4" s="1">
+      <c r="H4" s="3">
         <v>44283</v>
       </c>
-      <c r="I4" s="1">
+      <c r="I4" s="3">
         <v>44282</v>
       </c>
       <c r="J4" t="s">
         <v>16</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>55</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -672,15 +618,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="6" max="6" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.28515625" customWidth="1"/>
+    <col min="5" max="5" width="41.85546875" customWidth="1"/>
+    <col min="6" max="6" width="27.85546875" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -699,7 +647,7 @@
       <c r="E1" t="s">
         <v>24</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="3" t="s">
         <v>25</v>
       </c>
     </row>
@@ -719,110 +667,10 @@
       <c r="E2" t="s">
         <v>29</v>
       </c>
-      <c r="F2" s="1">
+      <c r="F2" s="3">
         <v>44226</v>
       </c>
       <c r="G2" s="1"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E3" t="s">
-        <v>33</v>
-      </c>
-      <c r="F3" s="1">
-        <v>44227</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C4" t="s">
-        <v>35</v>
-      </c>
-      <c r="D4" t="s">
-        <v>36</v>
-      </c>
-      <c r="E4" t="s">
-        <v>37</v>
-      </c>
-      <c r="F4" s="1">
-        <v>44231</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C5" t="s">
-        <v>39</v>
-      </c>
-      <c r="D5" t="s">
-        <v>40</v>
-      </c>
-      <c r="E5" t="s">
-        <v>41</v>
-      </c>
-      <c r="F5" s="1">
-        <v>44233</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>42</v>
-      </c>
-      <c r="C6" t="s">
-        <v>43</v>
-      </c>
-      <c r="D6" t="s">
-        <v>44</v>
-      </c>
-      <c r="E6" t="s">
-        <v>45</v>
-      </c>
-      <c r="F6" s="1">
-        <v>44309</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>46</v>
-      </c>
-      <c r="C7" t="s">
-        <v>47</v>
-      </c>
-      <c r="D7" t="s">
-        <v>48</v>
-      </c>
-      <c r="E7" t="s">
-        <v>49</v>
-      </c>
-      <c r="F7" s="1">
-        <v>44311</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>